<commit_message>
For more stable Chrome Headless execution
</commit_message>
<xml_diff>
--- a/AzureDevOpsFriendlyArchhitecture/CreateNewBook/Main.rvl.xlsx
+++ b/AzureDevOpsFriendlyArchhitecture/CreateNewBook/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="43">
   <si>
     <t>Flow</t>
   </si>
@@ -127,6 +127,21 @@
   </si>
   <si>
     <t>Logout1</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>DoSleep</t>
+  </si>
+  <si>
+    <t>millis</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
 </sst>
 </file>
@@ -147,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="181">
+  <borders count="185">
     <border>
       <left/>
       <right/>
@@ -335,11 +350,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -521,6 +540,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="178" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="179" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="180" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="181" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="182" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="183" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="184" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,7 +553,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H44"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.86328125" customWidth="true"/>
@@ -663,129 +686,127 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="164" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="184"/>
       <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="164" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="165" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="8">
+      <c r="A8" s="165" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="166" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="166" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
         <v>22</v>
       </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="167" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="167" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>12</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="168" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="11">
+      <c r="A11" s="168" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="169" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -801,437 +822,523 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="170" t="s">
-        <v>7</v>
-      </c>
+      <c r="A12" s="181"/>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="169" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="182"/>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="170" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="171" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="171" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
         <v>27</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D16" t="s">
         <v>10</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E16" t="s">
         <v>11</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F16" t="s">
         <v>12</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="172" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="17">
+      <c r="A17" s="172" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
         <v>29</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
         <v>30</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E17" t="s">
         <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="173" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="174" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="175" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>17</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
       </c>
       <c r="G17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="173" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="174" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="183"/>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="175" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="176" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
+    <row r="22">
+      <c r="A22" s="176" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
         <v>28</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D22" t="s">
         <v>20</v>
       </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="177" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="177" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
         <v>22</v>
       </c>
-      <c r="E19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="178" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="178" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
         <v>24</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F24" t="s">
         <v>12</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="179" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
+    <row r="25">
+      <c r="A25" s="179" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
         <v>36</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="180" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="180" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D26" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="24"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="25"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="32"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="33"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="40"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="41"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="48"/>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="56"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="24"/>
     </row>
     <row r="28">
-      <c r="A28" s="57"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="64"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="32"/>
     </row>
     <row r="29">
-      <c r="A29" s="65"/>
-      <c r="B29" s="66"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="72"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="40"/>
     </row>
     <row r="30">
-      <c r="A30" s="73"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="80"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="48"/>
     </row>
     <row r="31">
-      <c r="A31" s="81"/>
-      <c r="B31" s="82"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="84"/>
-      <c r="E31" s="85"/>
-      <c r="F31" s="86"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="88"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="56"/>
     </row>
     <row r="32">
-      <c r="A32" s="89"/>
-      <c r="B32" s="90"/>
-      <c r="C32" s="91"/>
-      <c r="D32" s="92"/>
-      <c r="E32" s="93"/>
-      <c r="F32" s="94"/>
-      <c r="G32" s="95"/>
-      <c r="H32" s="96"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="64"/>
     </row>
     <row r="33">
-      <c r="A33" s="97"/>
-      <c r="B33" s="98"/>
-      <c r="C33" s="99"/>
-      <c r="D33" s="100"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="102"/>
-      <c r="G33" s="103"/>
-      <c r="H33" s="104"/>
+      <c r="A33" s="65"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="72"/>
     </row>
     <row r="34">
-      <c r="A34" s="105"/>
-      <c r="B34" s="106"/>
-      <c r="C34" s="107"/>
-      <c r="D34" s="108"/>
-      <c r="E34" s="109"/>
-      <c r="F34" s="110"/>
-      <c r="G34" s="111"/>
-      <c r="H34" s="112"/>
+      <c r="A34" s="73"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="79"/>
+      <c r="H34" s="80"/>
     </row>
     <row r="35">
-      <c r="A35" s="113"/>
-      <c r="B35" s="114"/>
-      <c r="C35" s="115"/>
-      <c r="D35" s="116"/>
-      <c r="E35" s="117"/>
-      <c r="F35" s="118"/>
-      <c r="G35" s="119"/>
-      <c r="H35" s="120"/>
+      <c r="A35" s="81"/>
+      <c r="B35" s="82"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="87"/>
+      <c r="H35" s="88"/>
     </row>
     <row r="36">
-      <c r="A36" s="121"/>
-      <c r="B36" s="122"/>
-      <c r="C36" s="123"/>
-      <c r="D36" s="124"/>
-      <c r="E36" s="125"/>
-      <c r="F36" s="126"/>
-      <c r="G36" s="127"/>
-      <c r="H36" s="128"/>
+      <c r="A36" s="89"/>
+      <c r="B36" s="90"/>
+      <c r="C36" s="91"/>
+      <c r="D36" s="92"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="95"/>
+      <c r="H36" s="96"/>
     </row>
     <row r="37">
-      <c r="A37" s="129"/>
-      <c r="B37" s="130"/>
-      <c r="C37" s="131"/>
-      <c r="D37" s="132"/>
-      <c r="E37" s="133"/>
-      <c r="F37" s="134"/>
-      <c r="G37" s="135"/>
-      <c r="H37" s="136"/>
+      <c r="A37" s="97"/>
+      <c r="B37" s="98"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="101"/>
+      <c r="F37" s="102"/>
+      <c r="G37" s="103"/>
+      <c r="H37" s="104"/>
     </row>
     <row r="38">
-      <c r="A38" s="137"/>
-      <c r="B38" s="138"/>
-      <c r="C38" s="139"/>
-      <c r="D38" s="140"/>
-      <c r="E38" s="141"/>
-      <c r="F38" s="142"/>
-      <c r="G38" s="143"/>
-      <c r="H38" s="144"/>
+      <c r="A38" s="105"/>
+      <c r="B38" s="106"/>
+      <c r="C38" s="107"/>
+      <c r="D38" s="108"/>
+      <c r="E38" s="109"/>
+      <c r="F38" s="110"/>
+      <c r="G38" s="111"/>
+      <c r="H38" s="112"/>
     </row>
     <row r="39">
-      <c r="A39" s="145"/>
-      <c r="B39" s="146"/>
-      <c r="C39" s="147"/>
-      <c r="D39" s="148"/>
-      <c r="E39" s="149"/>
-      <c r="F39" s="150"/>
-      <c r="G39" s="151"/>
-      <c r="H39" s="152"/>
+      <c r="A39" s="113"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="115"/>
+      <c r="D39" s="116"/>
+      <c r="E39" s="117"/>
+      <c r="F39" s="118"/>
+      <c r="G39" s="119"/>
+      <c r="H39" s="120"/>
     </row>
     <row r="40">
-      <c r="A40" s="153"/>
-      <c r="B40" s="154"/>
-      <c r="C40" s="155"/>
-      <c r="D40" s="156"/>
-      <c r="E40" s="157"/>
-      <c r="F40" s="158"/>
-      <c r="G40" s="159"/>
-      <c r="H40" s="160"/>
+      <c r="A40" s="121"/>
+      <c r="B40" s="122"/>
+      <c r="C40" s="123"/>
+      <c r="D40" s="124"/>
+      <c r="E40" s="125"/>
+      <c r="F40" s="126"/>
+      <c r="G40" s="127"/>
+      <c r="H40" s="128"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="129"/>
+      <c r="B41" s="130"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="132"/>
+      <c r="E41" s="133"/>
+      <c r="F41" s="134"/>
+      <c r="G41" s="135"/>
+      <c r="H41" s="136"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="137"/>
+      <c r="B42" s="138"/>
+      <c r="C42" s="139"/>
+      <c r="D42" s="140"/>
+      <c r="E42" s="141"/>
+      <c r="F42" s="142"/>
+      <c r="G42" s="143"/>
+      <c r="H42" s="144"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="145"/>
+      <c r="B43" s="146"/>
+      <c r="C43" s="147"/>
+      <c r="D43" s="148"/>
+      <c r="E43" s="149"/>
+      <c r="F43" s="150"/>
+      <c r="G43" s="151"/>
+      <c r="H43" s="152"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="153"/>
+      <c r="B44" s="154"/>
+      <c r="C44" s="155"/>
+      <c r="D44" s="156"/>
+      <c r="E44" s="157"/>
+      <c r="F44" s="158"/>
+      <c r="G44" s="159"/>
+      <c r="H44" s="160"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>